<commit_message>
Correction of Table S3
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_3.xlsx
+++ b/SVGs/SupplTable_3.xlsx
@@ -417,7 +417,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -638,15 +638,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,16 +769,16 @@
   </sheetPr>
   <dimension ref="B1:U17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.92"/>
@@ -877,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="21" t="n">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="H5" s="22" t="n">
         <v>0</v>
@@ -887,7 +879,7 @@
       </c>
       <c r="J5" s="24" t="n">
         <f aca="false">SUM(G5:I5)</f>
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="10" t="s">
@@ -913,17 +905,17 @@
         <v>12</v>
       </c>
       <c r="G6" s="31" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="33" t="n">
         <f aca="false">SUM(G6:I6)</f>
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="L6" s="34" t="s">
         <v>12</v>
@@ -948,17 +940,17 @@
         <v>13</v>
       </c>
       <c r="G7" s="31" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H7" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="32" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J7" s="33" t="n">
         <f aca="false">SUM(G7:I7)</f>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="L7" s="34" t="s">
         <v>13</v>
@@ -983,17 +975,17 @@
         <v>14</v>
       </c>
       <c r="G8" s="39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="40" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="41" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J8" s="33" t="n">
         <f aca="false">SUM(G8:I8)</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="42" t="s">
@@ -1023,17 +1015,17 @@
         <v>4</v>
       </c>
       <c r="G9" s="49" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="50" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I9" s="51" t="n">
-        <v>695</v>
+        <v>0</v>
       </c>
       <c r="J9" s="52" t="n">
         <f aca="false">SUM(G9:I9)</f>
-        <v>709</v>
+        <v>0</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="53"/>
@@ -1062,7 +1054,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="21" t="n">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="H10" s="22" t="n">
         <v>0</v>
@@ -1072,7 +1064,7 @@
       </c>
       <c r="J10" s="54" t="n">
         <f aca="false">SUM(G10:I10)</f>
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="53"/>
@@ -1095,17 +1087,17 @@
         <v>12</v>
       </c>
       <c r="G11" s="31" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="H11" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="55" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" s="33" t="n">
         <f aca="false">SUM(G11:I11)</f>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="53"/>
@@ -1128,17 +1120,17 @@
         <v>13</v>
       </c>
       <c r="G12" s="31" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="32" t="n">
-        <v>7</v>
-      </c>
-      <c r="J12" s="55" t="n">
+        <v>20</v>
+      </c>
+      <c r="J12" s="33" t="n">
         <f aca="false">SUM(G12:I12)</f>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="53"/>
@@ -1161,17 +1153,17 @@
         <v>14</v>
       </c>
       <c r="G13" s="39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="40" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="56" t="n">
+        <v>16</v>
+      </c>
+      <c r="J13" s="55" t="n">
         <f aca="false">SUM(G13:I13)</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="53"/>
@@ -1196,17 +1188,17 @@
         <v>4</v>
       </c>
       <c r="G14" s="49" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="50" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I14" s="51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="57" t="n">
+        <v>695</v>
+      </c>
+      <c r="J14" s="52" t="n">
         <f aca="false">SUM(G14:I14)</f>
-        <v>0</v>
+        <v>709</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="53"/>
@@ -1221,7 +1213,7 @@
       <c r="U14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="58" t="s">
+      <c r="F15" s="56" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="40" t="n">
@@ -1236,33 +1228,33 @@
         <f aca="false">SUM(I5:I14)</f>
         <v>743</v>
       </c>
-      <c r="J15" s="59" t="n">
+      <c r="J15" s="57" t="n">
         <f aca="false">SUM(G15:I15)</f>
         <v>884</v>
       </c>
-      <c r="M15" s="60"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="61"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="59"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M16" s="63" t="s">
+      <c r="M16" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L17" s="65"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="68" t="s">
+      <c r="L17" s="63"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="69"/>
+      <c r="P17" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>